<commit_message>
Removed 16.5ohm electromagnet resistors
</commit_message>
<xml_diff>
--- a/BOM/MSB_v1.0_Jan2023.xlsx
+++ b/BOM/MSB_v1.0_Jan2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\MSB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F168DF50-B35F-40B2-A323-520F43DC9BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152D492-C7A4-4190-9E4E-942E093808E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CB5471BA-2E76-4134-80E3-6C9BC67DDA87}"/>
   </bookViews>
@@ -738,14 +738,17 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="19" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
     <col min="5" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="8" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>